<commit_message>
business analysis updated (name adjustment)
</commit_message>
<xml_diff>
--- a/docs/analysis/KostenNutzenAnalyse.xlsx
+++ b/docs/analysis/KostenNutzenAnalyse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="0" windowWidth="18870" windowHeight="13200"/>
+    <workbookView xWindow="5100" yWindow="0" windowWidth="18870" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
-    <t>Kosten-Nutzen-Analyse für Implementierung des Emotion Detectors von Shiretech Inc.</t>
-  </si>
-  <si>
     <t>Kosten</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Monat</t>
+  </si>
+  <si>
+    <t>Kosten-Nutzen-Analyse für Implementierung des ShireEyes von Shiretech Inc.</t>
   </si>
 </sst>
 </file>
@@ -649,9 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -664,7 +662,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -678,33 +676,33 @@
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -735,7 +733,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -766,13 +764,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="15">
         <v>50000</v>
@@ -800,13 +798,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="15">
         <v>20000</v>
@@ -834,13 +832,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="15">
         <v>50</v>
@@ -868,13 +866,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15">
         <v>45</v>
@@ -902,7 +900,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -933,13 +931,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="15">
         <v>1500</v>
@@ -967,13 +965,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="15">
         <v>50</v>
@@ -1001,13 +999,13 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="19">
         <v>5</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="21">
         <v>80</v>
@@ -1036,33 +1034,33 @@
     <row r="13" spans="1:9" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1093,7 +1091,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
@@ -1123,13 +1121,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="11">
         <v>0.1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="15">
         <v>4500</v>
@@ -1157,13 +1155,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2">
         <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="15">
         <v>40</v>
@@ -1191,13 +1189,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="15">
         <v>30</v>
@@ -1225,7 +1223,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
@@ -1241,13 +1239,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="11">
         <v>-0.15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="15">
         <v>1500</v>
@@ -1275,7 +1273,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
@@ -1288,7 +1286,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -1301,7 +1299,7 @@
     </row>
     <row r="23" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>

</xml_diff>